<commit_message>
Change import trip from excel dates formats, view all trips to dd/MM/yyyy
</commit_message>
<xml_diff>
--- a/angular/src/assets/sampleFiles/Import_SAAS_Trip_details.xlsx
+++ b/angular/src/assets/sampleFiles/Import_SAAS_Trip_details.xlsx
@@ -38,14 +38,6 @@
 الرقم المرجعي للرحلة</t>
   </si>
   <si>
-    <t xml:space="preserve">Pick-up date start  (yyyy/MM/dd)
-تاريخ بداية التحميل </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pick-up date end  (yyyy/MM/dd)
-تاريخ نهاية التحميل </t>
-  </si>
-  <si>
     <t xml:space="preserve">Approximate total value of goods
 القيمة التقريبة للبضاعة </t>
   </si>
@@ -134,6 +126,14 @@
   </si>
   <si>
     <t>Detergents</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pick-up date start  (dd/MM/yyyy)
+تاريخ بداية التحميل </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pick-up date end  (dd/MM/yyyy)
+تاريخ نهاية التحميل </t>
   </si>
 </sst>
 </file>
@@ -592,8 +592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -616,49 +616,49 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" s="2" t="s">
+      <c r="N1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:16" s="4" customFormat="1" ht="15" customHeight="1">
@@ -842,67 +842,67 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="15" thickBot="1">
       <c r="A8" s="9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="15" thickBot="1">
       <c r="A9" s="10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="15" thickBot="1">
       <c r="A10" s="9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="15" thickBot="1">
       <c r="A11" s="10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Client name (shipper), shipper reference, booking #, container# - to excel sheet to upload trips
</commit_message>
<xml_diff>
--- a/angular/src/assets/sampleFiles/Import_SAAS_Trip_details.xlsx
+++ b/angular/src/assets/sampleFiles/Import_SAAS_Trip_details.xlsx
@@ -1,38 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10916"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\source\repos\tachyon-core1\angular\src\assets\sampleFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/islam/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35848FCA-0508-DE4B-9E3A-16B7D52F12D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="0" yWindow="860" windowWidth="34200" windowHeight="20180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Lists" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Trip Reference No *  
 الرقم المرجعي للرحلة</t>
@@ -134,12 +123,24 @@
   <si>
     <t xml:space="preserve">Pick-up date end  (dd/MM/yyyy)
 تاريخ نهاية التحميل </t>
+  </si>
+  <si>
+    <t>Actor Shipper</t>
+  </si>
+  <si>
+    <t>Container Number</t>
+  </si>
+  <si>
+    <t>Shipper Reference</t>
+  </si>
+  <si>
+    <t>Booking number</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7">
     <font>
       <sz val="11"/>
@@ -589,29 +590,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P50"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:T50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="224" workbookViewId="0">
+      <selection activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="30.109375" customWidth="1"/>
+    <col min="1" max="1" width="30.1640625" customWidth="1"/>
     <col min="2" max="2" width="59.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="57.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="57.5" style="1" customWidth="1"/>
     <col min="4" max="4" width="51.33203125" customWidth="1"/>
-    <col min="5" max="5" width="27.5546875" customWidth="1"/>
+    <col min="5" max="5" width="27.5" customWidth="1"/>
     <col min="6" max="11" width="36.33203125" customWidth="1"/>
-    <col min="12" max="12" width="33.5546875" customWidth="1"/>
-    <col min="13" max="13" width="33.88671875" customWidth="1"/>
-    <col min="14" max="14" width="34.5546875" customWidth="1"/>
-    <col min="15" max="15" width="31.44140625" customWidth="1"/>
-    <col min="16" max="16" width="29.109375" customWidth="1"/>
+    <col min="12" max="12" width="33.5" customWidth="1"/>
+    <col min="13" max="13" width="33.83203125" customWidth="1"/>
+    <col min="14" max="14" width="34.5" customWidth="1"/>
+    <col min="15" max="15" width="31.5" customWidth="1"/>
+    <col min="16" max="16" width="29.1640625" customWidth="1"/>
+    <col min="17" max="17" width="15.5" customWidth="1"/>
+    <col min="18" max="18" width="15.83203125" customWidth="1"/>
+    <col min="19" max="19" width="15.5" customWidth="1"/>
+    <col min="20" max="20" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="3" customFormat="1" ht="20.399999999999999">
+    <row r="1" spans="1:20" s="3" customFormat="1" ht="24">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -660,68 +665,80 @@
       <c r="P1" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" s="4" customFormat="1" ht="15" customHeight="1">
+      <c r="Q1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1">
       <c r="B2" s="5"/>
       <c r="C2" s="6"/>
       <c r="N2" s="8"/>
       <c r="O2" s="8"/>
     </row>
-    <row r="3" spans="1:16" s="4" customFormat="1" ht="15" customHeight="1">
+    <row r="3" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1">
       <c r="B3" s="5"/>
       <c r="C3" s="6"/>
       <c r="N3" s="8"/>
       <c r="O3" s="8"/>
     </row>
-    <row r="4" spans="1:16" s="4" customFormat="1" ht="15" customHeight="1">
+    <row r="4" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1">
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
     </row>
-    <row r="5" spans="1:16" s="4" customFormat="1" ht="15" customHeight="1">
+    <row r="5" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1">
       <c r="B5" s="6"/>
       <c r="C5" s="7"/>
     </row>
-    <row r="6" spans="1:16" s="4" customFormat="1" ht="15" customHeight="1">
+    <row r="6" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1">
       <c r="B6" s="6"/>
       <c r="C6" s="7"/>
     </row>
-    <row r="7" spans="1:16" s="4" customFormat="1" ht="15" customHeight="1">
+    <row r="7" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1">
       <c r="B7" s="6"/>
       <c r="C7" s="7"/>
     </row>
-    <row r="8" spans="1:16" s="4" customFormat="1" ht="15" customHeight="1">
+    <row r="8" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1">
       <c r="B8" s="6"/>
       <c r="C8" s="7"/>
     </row>
-    <row r="9" spans="1:16" s="4" customFormat="1" ht="15" customHeight="1">
+    <row r="9" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1">
       <c r="B9" s="6"/>
       <c r="C9" s="7"/>
     </row>
-    <row r="10" spans="1:16" s="4" customFormat="1" ht="15" customHeight="1">
+    <row r="10" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1">
       <c r="B10" s="6"/>
       <c r="C10" s="7"/>
     </row>
-    <row r="11" spans="1:16" s="4" customFormat="1" ht="15" customHeight="1">
+    <row r="11" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1">
       <c r="B11" s="6"/>
       <c r="C11" s="7"/>
     </row>
-    <row r="12" spans="1:16" s="4" customFormat="1" ht="15" customHeight="1">
+    <row r="12" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1">
       <c r="B12" s="6"/>
       <c r="C12" s="7"/>
     </row>
-    <row r="13" spans="1:16" s="4" customFormat="1" ht="15" customHeight="1">
+    <row r="13" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1">
       <c r="B13" s="6"/>
       <c r="C13" s="7"/>
     </row>
-    <row r="14" spans="1:16" s="4" customFormat="1" ht="15" customHeight="1">
+    <row r="14" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1">
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
     </row>
-    <row r="15" spans="1:16" s="4" customFormat="1" ht="15" customHeight="1">
+    <row r="15" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1">
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
     </row>
-    <row r="16" spans="1:16" s="4" customFormat="1" ht="15" customHeight="1">
+    <row r="16" spans="1:20" s="4" customFormat="1" ht="15" customHeight="1">
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
     </row>
@@ -803,10 +820,10 @@
     <row r="50" ht="15" customHeight="1"/>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H31:I1048576 F1:G1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H31:I1048576 F1:G1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"yes,no"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H30">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H30" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Single Drop,Multiple Drops"</formula1>
     </dataValidation>
   </dataValidations>
@@ -815,7 +832,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
             <xm:f>Lists!$A$2:$A$13</xm:f>
           </x14:formula1>
@@ -828,16 +845,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -875,22 +892,22 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="15" thickBot="1">
+    <row r="8" spans="1:1" ht="16" thickBot="1">
       <c r="A8" s="9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="15" thickBot="1">
+    <row r="9" spans="1:1" ht="16" thickBot="1">
       <c r="A9" s="10" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="15" thickBot="1">
+    <row r="10" spans="1:1" ht="16" thickBot="1">
       <c r="A10" s="9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="15" thickBot="1">
+    <row r="11" spans="1:1" ht="16" thickBot="1">
       <c r="A11" s="10" t="s">
         <v>24</v>
       </c>

</xml_diff>